<commit_message>
Misc change in freight charge upload
</commit_message>
<xml_diff>
--- a/src/assets/Download/FreightChargeTemplate.xlsx
+++ b/src/assets/Download/FreightChargeTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>From</t>
   </si>
@@ -25,6 +25,9 @@
     <t>RateType</t>
   </si>
   <si>
+    <t>Capacity</t>
+  </si>
+  <si>
     <t>Rate</t>
   </si>
   <si>
@@ -32,6 +35,29 @@
   </si>
   <si>
     <t>TransportMode</t>
+  </si>
+  <si>
+    <t>SURAT</t>
+  </si>
+  <si>
+    <t>DELHI</t>
+  </si>
+  <si>
+    <t>Flat</t>
+  </si>
+  <si>
+    <t>Veh- 10 MT</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10.5"/>
+        <color theme="1"/>
+        <rFont val="helvetica"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Road</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -45,7 +71,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +80,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -65,6 +92,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
+      <name val="helvetica"/>
       <charset val="134"/>
     </font>
     <font>
@@ -547,137 +580,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -690,6 +723,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,23 +1259,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:F$1048576"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="7.57142857142857" style="2" customWidth="1"/>
-    <col min="2" max="2" width="4" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.28571428571429" style="2" customWidth="1"/>
     <col min="3" max="3" width="12.1428571428571" style="2" customWidth="1"/>
-    <col min="4" max="4" width="6.28571428571429" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15" style="3" customWidth="1"/>
-    <col min="6" max="6" width="18.7142857142857" style="2" customWidth="1"/>
+    <col min="4" max="4" width="9.71428571428571" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.28571428571429" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15" style="3" customWidth="1"/>
+    <col min="7" max="7" width="18.7142857142857" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:6">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1255,9 +1292,44 @@
       <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="3">
+        <v>100</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="7:7">
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="7:7">
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="7:7">
+      <c r="G5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Commited Changes Of Customer Contract
</commit_message>
<xml_diff>
--- a/src/assets/Download/FreightChargeTemplate.xlsx
+++ b/src/assets/Download/FreightChargeTemplate.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>From</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>TransportMode</t>
+  </si>
+  <si>
+    <t>ValidFromDate</t>
+  </si>
+  <si>
+    <t>ValidToDate</t>
   </si>
   <si>
     <t>SURAT</t>
@@ -59,17 +65,22 @@
       <t>Road</t>
     </r>
   </si>
+  <si>
+    <t>31/3/2024</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="181" formatCode="[$-409]dddd\,mmmm\ d\,yyyy;@"/>
+    <numFmt numFmtId="182" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -710,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -721,9 +732,16 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="181" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1259,13 +1277,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="7.57142857142857" style="2" customWidth="1"/>
     <col min="2" max="2" width="9.28571428571429" style="2" customWidth="1"/>
@@ -1274,43 +1292,51 @@
     <col min="5" max="5" width="6.28571428571429" style="3" customWidth="1"/>
     <col min="6" max="6" width="15" style="3" customWidth="1"/>
     <col min="7" max="7" width="18.7142857142857" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.1428571428571" style="4"/>
+    <col min="9" max="9" width="9.14285714285714" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:7">
-      <c r="A1" s="4" t="s">
+    <row r="1" s="1" customFormat="1" spans="1:9">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>100</v>
@@ -1318,18 +1344,24 @@
       <c r="F2" s="3">
         <v>1</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>11</v>
+      <c r="G2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="9">
+        <v>45294</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="7:7">
-      <c r="G3" s="6"/>
+      <c r="G3" s="8"/>
     </row>
     <row r="4" spans="7:7">
-      <c r="G4" s="6"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" spans="7:7">
-      <c r="G5" s="6"/>
+      <c r="G5" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>